<commit_message>
drop days on "the"; add "or equal"
</commit_message>
<xml_diff>
--- a/content/data/crew_food_prefs.xlsx
+++ b/content/data/crew_food_prefs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kvaleD1\Documents\RCAMP\R-camp-slides\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kvaleD1\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACAD8E24-29CC-478B-9B36-F2840015FBAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F3FBAFD-96B9-4323-9208-6DF93634F7DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="14136" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,9 +37,6 @@
     <t>egg_allergy</t>
   </si>
   <si>
-    <t>days_on_the_ship</t>
-  </si>
-  <si>
     <t>meals_per_day</t>
   </si>
   <si>
@@ -464,6 +461,9 @@
   </si>
   <si>
     <t>sugar</t>
+  </si>
+  <si>
+    <t>days_on_ship</t>
   </si>
 </sst>
 </file>
@@ -857,7 +857,7 @@
   <dimension ref="A2:H73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -882,24 +882,24 @@
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2">
         <v>45252</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -914,18 +914,18 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2">
         <v>45256</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -940,18 +940,18 @@
         <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2">
         <v>45248</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
@@ -966,18 +966,18 @@
         <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2">
         <v>45254</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -992,18 +992,18 @@
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="2">
         <v>45254</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" t="b">
         <v>1</v>
@@ -1018,18 +1018,18 @@
         <v>3</v>
       </c>
       <c r="H7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2">
         <v>45251</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" t="b">
         <v>1</v>
@@ -1044,18 +1044,18 @@
         <v>3</v>
       </c>
       <c r="H8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="2">
         <v>45254</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" t="b">
         <v>1</v>
@@ -1070,18 +1070,18 @@
         <v>3</v>
       </c>
       <c r="H9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="2">
         <v>45252</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
@@ -1096,18 +1096,18 @@
         <v>2</v>
       </c>
       <c r="H10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="2">
         <v>45255</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
@@ -1122,18 +1122,18 @@
         <v>2</v>
       </c>
       <c r="H11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="2">
         <v>45254</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" t="b">
         <v>1</v>
@@ -1148,18 +1148,18 @@
         <v>3</v>
       </c>
       <c r="H12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="2">
         <v>45249</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
@@ -1174,18 +1174,18 @@
         <v>4</v>
       </c>
       <c r="H13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="2">
         <v>45253</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" t="b">
         <v>1</v>
@@ -1200,18 +1200,18 @@
         <v>3</v>
       </c>
       <c r="H14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="2">
         <v>45249</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" t="b">
         <v>0</v>
@@ -1226,18 +1226,18 @@
         <v>3</v>
       </c>
       <c r="H15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="2">
         <v>45253</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D16" t="b">
         <v>1</v>
@@ -1252,18 +1252,18 @@
         <v>4</v>
       </c>
       <c r="H16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17" s="2">
         <v>45251</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D17" t="b">
         <v>1</v>
@@ -1278,18 +1278,18 @@
         <v>2</v>
       </c>
       <c r="H17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" s="2">
         <v>45256</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D18" t="b">
         <v>1</v>
@@ -1304,18 +1304,18 @@
         <v>4</v>
       </c>
       <c r="H18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B19" s="2">
         <v>45256</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D19" t="b">
         <v>1</v>
@@ -1330,18 +1330,18 @@
         <v>4</v>
       </c>
       <c r="H19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" s="2">
         <v>45253</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" t="b">
         <v>1</v>
@@ -1356,18 +1356,18 @@
         <v>2</v>
       </c>
       <c r="H20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B21" s="2">
         <v>45255</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" t="b">
         <v>1</v>
@@ -1382,18 +1382,18 @@
         <v>2</v>
       </c>
       <c r="H21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22" s="2">
         <v>45250</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D22" t="b">
         <v>1</v>
@@ -1408,18 +1408,18 @@
         <v>3</v>
       </c>
       <c r="H22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B23" s="2">
         <v>45247</v>
       </c>
       <c r="C23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D23" t="b">
         <v>1</v>
@@ -1434,18 +1434,18 @@
         <v>2</v>
       </c>
       <c r="H23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24" s="2">
         <v>45254</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D24" t="b">
         <v>1</v>
@@ -1460,18 +1460,18 @@
         <v>3</v>
       </c>
       <c r="H24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B25" s="2">
         <v>45250</v>
       </c>
       <c r="C25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D25" t="b">
         <v>1</v>
@@ -1486,18 +1486,18 @@
         <v>3</v>
       </c>
       <c r="H25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26" s="2">
         <v>45254</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D26" t="b">
         <v>1</v>
@@ -1512,18 +1512,18 @@
         <v>3</v>
       </c>
       <c r="H26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" s="2">
         <v>45256</v>
       </c>
       <c r="C27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D27" t="b">
         <v>1</v>
@@ -1538,18 +1538,18 @@
         <v>4</v>
       </c>
       <c r="H27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B28" s="2">
         <v>45254</v>
       </c>
       <c r="C28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D28" t="b">
         <v>1</v>
@@ -1564,18 +1564,18 @@
         <v>3</v>
       </c>
       <c r="H28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B29" s="2">
         <v>45255</v>
       </c>
       <c r="C29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D29" t="b">
         <v>1</v>
@@ -1590,18 +1590,18 @@
         <v>3</v>
       </c>
       <c r="H29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B30" s="2">
         <v>45247</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D30" t="b">
         <v>1</v>
@@ -1616,18 +1616,18 @@
         <v>4</v>
       </c>
       <c r="H30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B31" s="2">
         <v>45256</v>
       </c>
       <c r="C31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D31" t="b">
         <v>0</v>
@@ -1642,18 +1642,18 @@
         <v>2</v>
       </c>
       <c r="H31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B32" s="2">
         <v>45256</v>
       </c>
       <c r="C32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D32" t="b">
         <v>1</v>
@@ -1668,18 +1668,18 @@
         <v>3</v>
       </c>
       <c r="H32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B33" s="2">
         <v>45253</v>
       </c>
       <c r="C33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D33" t="b">
         <v>1</v>
@@ -1694,18 +1694,18 @@
         <v>4</v>
       </c>
       <c r="H33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B34" s="2">
         <v>45249</v>
       </c>
       <c r="C34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D34" t="b">
         <v>1</v>
@@ -1720,18 +1720,18 @@
         <v>4</v>
       </c>
       <c r="H34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B35" s="2">
         <v>45251</v>
       </c>
       <c r="C35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D35" t="b">
         <v>1</v>
@@ -1746,18 +1746,18 @@
         <v>4</v>
       </c>
       <c r="H35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B36" s="2">
         <v>45251</v>
       </c>
       <c r="C36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D36" t="b">
         <v>1</v>
@@ -1772,18 +1772,18 @@
         <v>4</v>
       </c>
       <c r="H36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B37" s="2">
         <v>45248</v>
       </c>
       <c r="C37" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D37" t="b">
         <v>1</v>
@@ -1798,18 +1798,18 @@
         <v>3</v>
       </c>
       <c r="H37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B38" s="2">
         <v>45251</v>
       </c>
       <c r="C38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D38" t="b">
         <v>1</v>
@@ -1824,18 +1824,18 @@
         <v>3</v>
       </c>
       <c r="H38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B39" s="2">
         <v>45256</v>
       </c>
       <c r="C39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D39" t="b">
         <v>1</v>
@@ -1850,18 +1850,18 @@
         <v>2</v>
       </c>
       <c r="H39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B40" s="2">
         <v>45253</v>
       </c>
       <c r="C40" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D40" t="b">
         <v>1</v>
@@ -1876,18 +1876,18 @@
         <v>3</v>
       </c>
       <c r="H40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B41" s="2">
         <v>45248</v>
       </c>
       <c r="C41" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D41" t="b">
         <v>1</v>
@@ -1902,18 +1902,18 @@
         <v>2</v>
       </c>
       <c r="H41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B42" s="2">
         <v>45255</v>
       </c>
       <c r="C42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D42" t="b">
         <v>1</v>
@@ -1928,18 +1928,18 @@
         <v>2</v>
       </c>
       <c r="H42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B43" s="2">
         <v>45254</v>
       </c>
       <c r="C43" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D43" t="b">
         <v>1</v>
@@ -1954,18 +1954,18 @@
         <v>2</v>
       </c>
       <c r="H43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B44" s="2">
         <v>45253</v>
       </c>
       <c r="C44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D44" t="b">
         <v>1</v>
@@ -1980,18 +1980,18 @@
         <v>3</v>
       </c>
       <c r="H44" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B45" s="2">
         <v>45254</v>
       </c>
       <c r="C45" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D45" t="b">
         <v>1</v>
@@ -2006,18 +2006,18 @@
         <v>4</v>
       </c>
       <c r="H45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B46" s="2">
         <v>45256</v>
       </c>
       <c r="C46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D46" t="b">
         <v>1</v>
@@ -2032,18 +2032,18 @@
         <v>2</v>
       </c>
       <c r="H46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B47" s="2">
         <v>45253</v>
       </c>
       <c r="C47" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D47" t="b">
         <v>1</v>
@@ -2058,18 +2058,18 @@
         <v>3</v>
       </c>
       <c r="H47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B48" s="2">
         <v>45248</v>
       </c>
       <c r="C48" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D48" t="b">
         <v>1</v>
@@ -2084,18 +2084,18 @@
         <v>4</v>
       </c>
       <c r="H48" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B49" s="2">
         <v>45254</v>
       </c>
       <c r="C49" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D49" t="b">
         <v>1</v>
@@ -2110,18 +2110,18 @@
         <v>2</v>
       </c>
       <c r="H49" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B50" s="2">
         <v>45252</v>
       </c>
       <c r="C50" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D50" t="b">
         <v>1</v>
@@ -2136,18 +2136,18 @@
         <v>3</v>
       </c>
       <c r="H50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B51" s="2">
         <v>45251</v>
       </c>
       <c r="C51" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D51" t="b">
         <v>1</v>
@@ -2162,18 +2162,18 @@
         <v>2</v>
       </c>
       <c r="H51" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B52" s="2">
         <v>45256</v>
       </c>
       <c r="C52" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D52" t="b">
         <v>1</v>
@@ -2188,18 +2188,18 @@
         <v>3</v>
       </c>
       <c r="H52" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B53" s="2">
         <v>45256</v>
       </c>
       <c r="C53" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D53" t="b">
         <v>1</v>
@@ -2214,18 +2214,18 @@
         <v>4</v>
       </c>
       <c r="H53" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B54" s="2">
         <v>45253</v>
       </c>
       <c r="C54" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D54" t="b">
         <v>1</v>
@@ -2240,18 +2240,18 @@
         <v>2</v>
       </c>
       <c r="H54" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B55" s="2">
         <v>45252</v>
       </c>
       <c r="C55" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D55" t="b">
         <v>1</v>
@@ -2266,18 +2266,18 @@
         <v>4</v>
       </c>
       <c r="H55" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B56" s="2">
         <v>45255</v>
       </c>
       <c r="C56" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D56" t="b">
         <v>1</v>
@@ -2292,18 +2292,18 @@
         <v>2</v>
       </c>
       <c r="H56" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B57" s="2">
         <v>45249</v>
       </c>
       <c r="C57" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D57" t="b">
         <v>0</v>
@@ -2318,18 +2318,18 @@
         <v>3</v>
       </c>
       <c r="H57" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B58" s="2">
         <v>45250</v>
       </c>
       <c r="C58" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D58" t="b">
         <v>1</v>
@@ -2344,18 +2344,18 @@
         <v>3</v>
       </c>
       <c r="H58" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B59" s="2">
         <v>45248</v>
       </c>
       <c r="C59" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D59" t="b">
         <v>1</v>
@@ -2370,18 +2370,18 @@
         <v>4</v>
       </c>
       <c r="H59" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B60" s="2">
         <v>45251</v>
       </c>
       <c r="C60" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D60" t="b">
         <v>1</v>
@@ -2396,18 +2396,18 @@
         <v>4</v>
       </c>
       <c r="H60" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B61" s="2">
         <v>45252</v>
       </c>
       <c r="C61" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D61" t="b">
         <v>1</v>
@@ -2422,18 +2422,18 @@
         <v>2</v>
       </c>
       <c r="H61" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B62" s="2">
         <v>45254</v>
       </c>
       <c r="C62" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D62" t="b">
         <v>1</v>
@@ -2448,18 +2448,18 @@
         <v>2</v>
       </c>
       <c r="H62" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B63" s="2">
         <v>45255</v>
       </c>
       <c r="C63" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D63" t="b">
         <v>1</v>
@@ -2474,18 +2474,18 @@
         <v>3</v>
       </c>
       <c r="H63" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B64" s="2">
         <v>45247</v>
       </c>
       <c r="C64" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D64" t="b">
         <v>1</v>
@@ -2500,18 +2500,18 @@
         <v>4</v>
       </c>
       <c r="H64" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B65" s="2">
         <v>45256</v>
       </c>
       <c r="C65" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D65" t="b">
         <v>1</v>
@@ -2526,18 +2526,18 @@
         <v>4</v>
       </c>
       <c r="H65" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B66" s="2">
         <v>45250</v>
       </c>
       <c r="C66" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D66" t="b">
         <v>1</v>
@@ -2552,18 +2552,18 @@
         <v>3</v>
       </c>
       <c r="H66" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B67" s="2">
         <v>45248</v>
       </c>
       <c r="C67" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D67" t="b">
         <v>1</v>
@@ -2578,18 +2578,18 @@
         <v>2</v>
       </c>
       <c r="H67" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B68" s="2">
         <v>45253</v>
       </c>
       <c r="C68" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D68" t="b">
         <v>1</v>
@@ -2604,18 +2604,18 @@
         <v>2</v>
       </c>
       <c r="H68" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B69" s="2">
         <v>45249</v>
       </c>
       <c r="C69" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D69" t="b">
         <v>1</v>
@@ -2630,18 +2630,18 @@
         <v>4</v>
       </c>
       <c r="H69" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B70" s="2">
         <v>45249</v>
       </c>
       <c r="C70" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D70" t="b">
         <v>1</v>
@@ -2656,18 +2656,18 @@
         <v>3</v>
       </c>
       <c r="H70" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B71" s="2">
         <v>45253</v>
       </c>
       <c r="C71" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D71" t="b">
         <v>1</v>
@@ -2682,18 +2682,18 @@
         <v>3</v>
       </c>
       <c r="H71" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B72" s="2">
         <v>45248</v>
       </c>
       <c r="C72" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D72" t="b">
         <v>1</v>
@@ -2708,18 +2708,18 @@
         <v>4</v>
       </c>
       <c r="H72" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B73" s="2">
         <v>2</v>
       </c>
       <c r="C73" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F73">
         <v>1000</v>
@@ -2728,7 +2728,7 @@
         <v>100</v>
       </c>
       <c r="H73" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>